<commit_message>
updating terms and imports
</commit_message>
<xml_diff>
--- a/terms/bodyTerms.xlsx
+++ b/terms/bodyTerms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8E0479-0C8F-C847-8A92-92CC7E687108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219BE285-0A03-A544-8B32-AD068F892D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="8320" xr2:uid="{48D2B3CD-A9E9-BF44-92BF-C9ED0F451C00}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBA_VT1000425</t>
+  </si>
+  <si>
+    <t>in FOVT</t>
+  </si>
+  <si>
+    <t>chest circumference</t>
   </si>
 </sst>
 </file>
@@ -722,7 +728,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +767,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>46</v>
@@ -773,7 +779,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -788,7 +794,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -808,7 +814,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -845,7 +851,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -882,11 +888,16 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="I9" s="4"/>

</xml_diff>